<commit_message>
Adding Notes to Lab 28. It Also Cannot Be Finished.
</commit_message>
<xml_diff>
--- a/28_mirtral_stenosis/mitral_stenosis_data.xlsx
+++ b/28_mirtral_stenosis/mitral_stenosis_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Time</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>(10 mins)</t>
+  </si>
+  <si>
+    <t>Once again, HumMod can only change the open areas by a tenth of a mm^2. This is counterproductive and will not permit this lab to be finished at current.</t>
   </si>
 </sst>
 </file>
@@ -165,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -194,6 +197,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:D26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -815,8 +821,26 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A30:M30"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="D3:D4"/>
@@ -825,7 +849,7 @@
     <mergeCell ref="D17:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Adding Some HumMod data and notes to Lab 28. Suspect that mitral stenosis is a stub in HumMod. No changes of note are ocurring.
</commit_message>
<xml_diff>
--- a/28_mirtral_stenosis/mitral_stenosis_data.xlsx
+++ b/28_mirtral_stenosis/mitral_stenosis_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="24">
   <si>
     <t>Time</t>
   </si>
@@ -73,6 +73,21 @@
   </si>
   <si>
     <t>Once again, HumMod can only change the open areas by a tenth of a mm^2. This is counterproductive and will not permit this lab to be finished at current.</t>
+  </si>
+  <si>
+    <t>The necessary changes to DES files for this lab to be completed have been made locally. The changes are available under a subdirectory in the labs folder of the HumMod github pages</t>
+  </si>
+  <si>
+    <t>HumMod</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>Hilariously enough, the changes to the mitral valve are not actually doing anything to the program. Shows me right for taking the initiative.</t>
+  </si>
+  <si>
+    <t>Suspect Mitral Stenosis is a Stub</t>
   </si>
 </sst>
 </file>
@@ -168,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -186,6 +201,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -199,8 +220,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,45 +520,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:N30"/>
+  <dimension ref="A2:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="7" t="s">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="10"/>
+      <c r="F3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30.75" thickBot="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+      <c r="D4" s="12"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="12"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -546,8 +599,16 @@
       <c r="D5" s="5">
         <v>5329</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5">
+        <v>5468</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -560,8 +621,18 @@
       <c r="D6" s="5">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="5">
+        <v>13.3</v>
+      </c>
+      <c r="H6" s="5">
+        <v>13</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -574,8 +645,16 @@
       <c r="D7" s="5">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F7" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -588,8 +667,16 @@
       <c r="D8" s="5">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -602,8 +689,16 @@
       <c r="D9" s="5">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F9" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -616,8 +711,16 @@
       <c r="D10" s="5">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="5">
+        <v>28</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
@@ -630,8 +733,16 @@
       <c r="D11" s="5">
         <v>91</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="5">
+        <v>93</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>11</v>
       </c>
@@ -644,8 +755,18 @@
       <c r="D12" s="5">
         <v>5414</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5">
+        <v>5421</v>
+      </c>
+      <c r="H12" s="5">
+        <v>5421</v>
+      </c>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -658,38 +779,76 @@
       <c r="D13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="F13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1">
+      <c r="F15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="11" t="s">
         <v>3</v>
       </c>
+      <c r="F17" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="30.75" thickBot="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="12"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" thickBot="1">
       <c r="A19" s="6" t="s">
@@ -704,6 +863,14 @@
       <c r="D19" s="5">
         <v>5314</v>
       </c>
+      <c r="F19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5">
+        <v>5468</v>
+      </c>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:14" ht="15.75" thickBot="1">
       <c r="A20" s="6" t="s">
@@ -718,6 +885,14 @@
       <c r="D20" s="5">
         <v>13</v>
       </c>
+      <c r="F20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="5">
+        <v>13.3</v>
+      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1">
       <c r="A21" s="6" t="s">
@@ -732,6 +907,14 @@
       <c r="D21" s="5">
         <v>10</v>
       </c>
+      <c r="F21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="5">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:14" ht="15.75" thickBot="1">
       <c r="A22" s="6" t="s">
@@ -746,6 +929,14 @@
       <c r="D22" s="5">
         <v>6.9</v>
       </c>
+      <c r="F22" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="5">
+        <v>6.2</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:14" ht="15.75" thickBot="1">
       <c r="A23" s="6" t="s">
@@ -760,6 +951,14 @@
       <c r="D23" s="5">
         <v>4.8</v>
       </c>
+      <c r="F23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1">
       <c r="A24" s="6" t="s">
@@ -774,6 +973,14 @@
       <c r="D24" s="5">
         <v>28</v>
       </c>
+      <c r="F24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="5">
+        <v>28</v>
+      </c>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:14" ht="15.75" thickBot="1">
       <c r="A25" s="6" t="s">
@@ -788,6 +995,14 @@
       <c r="D25" s="5">
         <v>91</v>
       </c>
+      <c r="F25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="5">
+        <v>93</v>
+      </c>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1">
       <c r="A26" s="6" t="s">
@@ -802,44 +1017,137 @@
       <c r="D26" s="5">
         <v>5415</v>
       </c>
+      <c r="F26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="5">
+        <v>5421</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:14" ht="15.75">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
+      <c r="N28" s="15"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75">
+      <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:14">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="15">
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A32:I33"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="I17:I18"/>
     <mergeCell ref="A30:M30"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>

</xml_diff>